<commit_message>
Stay Places edit added. Etc.
</commit_message>
<xml_diff>
--- a/box/1.xlsx
+++ b/box/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\wamp64\www\box\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B053EB7-E9C7-49A8-8224-E0EBA5E02F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03795057-D953-42D2-8C79-DF7D1C7E410E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8337" uniqueCount="5191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8350" uniqueCount="5191">
   <si>
     <t>1NMONTH_DB</t>
   </si>
@@ -16284,7 +16284,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -16983,6 +16983,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -17866,8 +17871,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:FR42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="FF37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="FP41" sqref="FP41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18010,7 +18015,7 @@
     <col min="158" max="158" width="30.7109375" customWidth="1"/>
     <col min="159" max="159" width="31.28515625" customWidth="1"/>
     <col min="160" max="160" width="33.5703125" customWidth="1"/>
-    <col min="161" max="161" width="27.5703125" customWidth="1"/>
+    <col min="161" max="161" width="27.5703125" style="139" customWidth="1"/>
     <col min="162" max="162" width="20" customWidth="1"/>
     <col min="163" max="163" width="18.28515625" customWidth="1"/>
     <col min="164" max="164" width="21" customWidth="1"/>
@@ -18352,7 +18357,7 @@
       <c r="FD1" s="2" t="s">
         <v>4881</v>
       </c>
-      <c r="FE1" s="2" t="s">
+      <c r="FE1" s="286" t="s">
         <v>4848</v>
       </c>
       <c r="FF1" s="2" t="s">
@@ -18471,6 +18476,7 @@
       <c r="EP2" s="85"/>
       <c r="EY2" s="192"/>
       <c r="EZ2" s="255"/>
+      <c r="FE2" s="286"/>
     </row>
     <row r="3" spans="1:174" s="2" customFormat="1">
       <c r="A3" s="1"/>
@@ -18550,6 +18556,7 @@
       <c r="EP3" s="85"/>
       <c r="EY3" s="192"/>
       <c r="EZ3" s="255"/>
+      <c r="FE3" s="286"/>
     </row>
     <row r="4" spans="1:174" s="2" customFormat="1">
       <c r="A4"/>
@@ -18629,6 +18636,7 @@
       <c r="EP4" s="85"/>
       <c r="EY4" s="192"/>
       <c r="EZ4" s="255"/>
+      <c r="FE4" s="286"/>
     </row>
     <row r="5" spans="1:174" ht="30">
       <c r="A5" s="65" t="s">
@@ -18954,7 +18962,7 @@
       <c r="FD5" s="1" t="s">
         <v>4924</v>
       </c>
-      <c r="FE5" s="152" t="s">
+      <c r="FE5" s="287" t="s">
         <v>4852</v>
       </c>
       <c r="FF5" s="152" t="s">
@@ -19697,7 +19705,7 @@
       <c r="FD7" s="31" t="s">
         <v>3928</v>
       </c>
-      <c r="FE7" s="31" t="s">
+      <c r="FE7" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF7" s="31" t="s">
@@ -20259,7 +20267,7 @@
       <c r="FD8" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE8" s="165" t="s">
+      <c r="FE8" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF8" s="165" t="s">
@@ -20786,7 +20794,7 @@
       <c r="FD9" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE9" s="165" t="s">
+      <c r="FE9" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF9" s="165" t="s">
@@ -21313,7 +21321,7 @@
       <c r="FD10" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE10" s="165" t="s">
+      <c r="FE10" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF10" s="165" t="s">
@@ -21840,7 +21848,7 @@
       <c r="FD11" s="244" t="s">
         <v>4917</v>
       </c>
-      <c r="FE11" s="235" t="s">
+      <c r="FE11" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF11" s="235" t="s">
@@ -22367,7 +22375,7 @@
       <c r="FD12" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE12" s="165" t="s">
+      <c r="FE12" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF12" s="165" t="s">
@@ -22894,7 +22902,7 @@
       <c r="FD13" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE13" s="165" t="s">
+      <c r="FE13" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF13" s="165" t="s">
@@ -23421,7 +23429,7 @@
       <c r="FD14" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE14" s="165" t="s">
+      <c r="FE14" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF14" s="165" t="s">
@@ -23948,7 +23956,7 @@
       <c r="FD15" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE15" s="165" t="s">
+      <c r="FE15" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF15" s="165" t="s">
@@ -24475,7 +24483,7 @@
       <c r="FD16" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE16" s="165" t="s">
+      <c r="FE16" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF16" s="165" t="s">
@@ -25002,7 +25010,7 @@
       <c r="FD17" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE17" s="165" t="s">
+      <c r="FE17" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF17" s="165" t="s">
@@ -25529,7 +25537,7 @@
       <c r="FD18" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE18" s="165" t="s">
+      <c r="FE18" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF18" s="165" t="s">
@@ -26056,7 +26064,7 @@
       <c r="FD19" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE19" s="165" t="s">
+      <c r="FE19" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF19" s="165" t="s">
@@ -26583,7 +26591,7 @@
       <c r="FD20" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE20" s="165" t="s">
+      <c r="FE20" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF20" s="165" t="s">
@@ -27110,7 +27118,7 @@
       <c r="FD21" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE21" s="165" t="s">
+      <c r="FE21" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF21" s="165" t="s">
@@ -27637,7 +27645,7 @@
       <c r="FD22" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE22" s="165" t="s">
+      <c r="FE22" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF22" s="165" t="s">
@@ -28164,7 +28172,7 @@
       <c r="FD23" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE23" s="165" t="s">
+      <c r="FE23" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF23" s="165" t="s">
@@ -28691,7 +28699,7 @@
       <c r="FD24" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE24" s="165" t="s">
+      <c r="FE24" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF24" s="165" t="s">
@@ -29218,7 +29226,7 @@
       <c r="FD25" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE25" s="165" t="s">
+      <c r="FE25" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF25" s="165" t="s">
@@ -29745,7 +29753,7 @@
       <c r="FD26" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE26" s="165" t="s">
+      <c r="FE26" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF26" s="165" t="s">
@@ -30272,7 +30280,7 @@
       <c r="FD27" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE27" s="165" t="s">
+      <c r="FE27" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF27" s="165" t="s">
@@ -30799,7 +30807,7 @@
       <c r="FD28" s="151" t="s">
         <v>4917</v>
       </c>
-      <c r="FE28" s="165" t="s">
+      <c r="FE28" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF28" s="165" t="s">
@@ -31322,7 +31330,7 @@
       <c r="FD29" s="215" t="s">
         <v>3928</v>
       </c>
-      <c r="FE29" s="206" t="s">
+      <c r="FE29" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF29" s="206" t="s">
@@ -31348,6 +31356,9 @@
       </c>
       <c r="FM29" s="206">
         <v>3</v>
+      </c>
+      <c r="FR29" s="165" t="s">
+        <v>4901</v>
       </c>
     </row>
     <row r="30" spans="1:174" s="60" customFormat="1" ht="90">
@@ -31842,7 +31853,7 @@
       <c r="FD30" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE30" s="165" t="s">
+      <c r="FE30" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF30" s="165" t="s">
@@ -31868,6 +31879,9 @@
       </c>
       <c r="FM30" s="165">
         <v>3</v>
+      </c>
+      <c r="FR30" s="165" t="s">
+        <v>4901</v>
       </c>
     </row>
     <row r="31" spans="1:174" s="60" customFormat="1" ht="90">
@@ -32362,7 +32376,7 @@
       <c r="FD31" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE31" s="165" t="s">
+      <c r="FE31" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF31" s="165" t="s">
@@ -32388,6 +32402,9 @@
       </c>
       <c r="FM31" s="165">
         <v>3</v>
+      </c>
+      <c r="FR31" s="165" t="s">
+        <v>4901</v>
       </c>
     </row>
     <row r="32" spans="1:174" s="60" customFormat="1" ht="90">
@@ -32882,7 +32899,7 @@
       <c r="FD32" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE32" s="165" t="s">
+      <c r="FE32" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF32" s="165" t="s">
@@ -32909,8 +32926,11 @@
       <c r="FM32" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR32" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="33" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A33" s="154" t="s">
         <v>2190</v>
       </c>
@@ -33402,7 +33422,7 @@
       <c r="FD33" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE33" s="165" t="s">
+      <c r="FE33" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF33" s="165" t="s">
@@ -33429,8 +33449,11 @@
       <c r="FM33" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR33" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="34" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A34" s="154" t="s">
         <v>2190</v>
       </c>
@@ -33922,7 +33945,7 @@
       <c r="FD34" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE34" s="165" t="s">
+      <c r="FE34" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF34" s="165" t="s">
@@ -33949,8 +33972,11 @@
       <c r="FM34" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR34" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A35" s="154" t="s">
         <v>2190</v>
       </c>
@@ -34442,7 +34468,7 @@
       <c r="FD35" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE35" s="165" t="s">
+      <c r="FE35" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF35" s="165" t="s">
@@ -34469,8 +34495,11 @@
       <c r="FM35" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR35" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A36" s="154" t="s">
         <v>2190</v>
       </c>
@@ -34962,7 +34991,7 @@
       <c r="FD36" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE36" s="165" t="s">
+      <c r="FE36" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF36" s="165" t="s">
@@ -34989,8 +35018,11 @@
       <c r="FM36" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR36" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A37" s="154" t="s">
         <v>2190</v>
       </c>
@@ -35482,7 +35514,7 @@
       <c r="FD37" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE37" s="165" t="s">
+      <c r="FE37" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF37" s="165" t="s">
@@ -35509,8 +35541,11 @@
       <c r="FM37" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR37" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A38" s="154" t="s">
         <v>2190</v>
       </c>
@@ -36002,7 +36037,7 @@
       <c r="FD38" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE38" s="165" t="s">
+      <c r="FE38" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF38" s="165" t="s">
@@ -36029,8 +36064,11 @@
       <c r="FM38" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR38" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A39" s="154" t="s">
         <v>2190</v>
       </c>
@@ -36522,7 +36560,7 @@
       <c r="FD39" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE39" s="165" t="s">
+      <c r="FE39" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF39" s="165" t="s">
@@ -36549,8 +36587,11 @@
       <c r="FM39" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:169" s="60" customFormat="1" ht="90">
+      <c r="FR39" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:174" s="60" customFormat="1" ht="90">
       <c r="A40" s="154" t="s">
         <v>2190</v>
       </c>
@@ -37042,7 +37083,7 @@
       <c r="FD40" s="151" t="s">
         <v>3928</v>
       </c>
-      <c r="FE40" s="165" t="s">
+      <c r="FE40" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF40" s="165" t="s">
@@ -37069,8 +37110,11 @@
       <c r="FM40" s="165">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:169" ht="90">
+      <c r="FR40" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:174" ht="90">
       <c r="A41" s="14" t="s">
         <v>2190</v>
       </c>
@@ -37420,7 +37464,7 @@
       <c r="FD41" s="150" t="s">
         <v>3928</v>
       </c>
-      <c r="FE41" s="55" t="s">
+      <c r="FE41" s="288" t="s">
         <v>4864</v>
       </c>
       <c r="FF41" s="55" t="s">
@@ -37447,8 +37491,11 @@
       <c r="FM41" s="55">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:169">
+      <c r="FR41" s="165" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="42" spans="1:174">
       <c r="DN42" s="262"/>
       <c r="DO42" s="135"/>
     </row>
@@ -68107,7 +68154,7 @@
       </c>
       <c r="F3" s="99">
         <f ca="1">TODAY()</f>
-        <v>45178</v>
+        <v>45179</v>
       </c>
       <c r="G3" s="97" t="str">
         <f ca="1">TEXT(F3,"ддММгггг")</f>

</xml_diff>